<commit_message>
added new tt with display function
</commit_message>
<xml_diff>
--- a/PBTT.xlsx
+++ b/PBTT.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23706"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23802"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3CC6CC8E-C483-4537-8A74-A3D033D1B098}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A66A9F89-F75E-4044-92D3-24ED00360E2D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="91">
   <si>
     <t>SUBJECT</t>
   </si>
@@ -51,15 +51,18 @@
     <t>TUESDAY</t>
   </si>
   <si>
+    <t>SATURDAY</t>
+  </si>
+  <si>
+    <t>IOTB</t>
+  </si>
+  <si>
+    <t>WEDNESDAY</t>
+  </si>
+  <si>
     <t>THURSDAY</t>
   </si>
   <si>
-    <t>IOTB</t>
-  </si>
-  <si>
-    <t>WEDNESDAY</t>
-  </si>
-  <si>
     <t>IOTC</t>
   </si>
   <si>
@@ -118,9 +121,6 @@
   </si>
   <si>
     <t>AIDAD</t>
-  </si>
-  <si>
-    <t>SATURDAY</t>
   </si>
   <si>
     <t>AIDBC</t>
@@ -660,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D127"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F127" sqref="F1:F127"/>
+    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="I102" sqref="I102:J115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -692,10 +692,10 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>810</v>
+        <v>855</v>
       </c>
       <c r="D2">
-        <v>870</v>
+        <v>915</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -706,10 +706,10 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>615</v>
+        <v>930</v>
       </c>
       <c r="D3">
-        <v>675</v>
+        <v>990</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -720,10 +720,10 @@
         <v>7</v>
       </c>
       <c r="C4">
-        <v>885</v>
+        <v>540</v>
       </c>
       <c r="D4">
-        <v>945</v>
+        <v>600</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -734,10 +734,10 @@
         <v>6</v>
       </c>
       <c r="C5">
-        <v>885</v>
+        <v>855</v>
       </c>
       <c r="D5">
-        <v>945</v>
+        <v>915</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -748,10 +748,10 @@
         <v>9</v>
       </c>
       <c r="C6">
-        <v>540</v>
+        <v>795</v>
       </c>
       <c r="D6">
-        <v>600</v>
+        <v>855</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -759,441 +759,441 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C7">
-        <v>690</v>
+        <v>855</v>
       </c>
       <c r="D7">
-        <v>750</v>
+        <v>915</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
       <c r="C8">
-        <v>885</v>
+        <v>855</v>
       </c>
       <c r="D8">
-        <v>945</v>
+        <v>915</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9">
-        <v>540</v>
+        <v>795</v>
       </c>
       <c r="D9">
-        <v>600</v>
+        <v>855</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C10">
-        <v>690</v>
+        <v>855</v>
       </c>
       <c r="D10">
-        <v>750</v>
+        <v>915</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
       </c>
       <c r="C11">
-        <v>810</v>
+        <v>855</v>
       </c>
       <c r="D11">
-        <v>870</v>
+        <v>915</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
       </c>
       <c r="C12">
-        <v>615</v>
+        <v>930</v>
       </c>
       <c r="D12">
-        <v>675</v>
+        <v>990</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
       </c>
       <c r="C13">
-        <v>885</v>
+        <v>540</v>
       </c>
       <c r="D13">
-        <v>945</v>
+        <v>600</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C14">
-        <v>810</v>
+        <v>855</v>
       </c>
       <c r="D14">
-        <v>870</v>
+        <v>915</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
-        <v>13</v>
-      </c>
       <c r="C15">
-        <v>810</v>
+        <v>855</v>
       </c>
       <c r="D15">
-        <v>870</v>
+        <v>915</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C16">
-        <v>810</v>
+        <v>855</v>
       </c>
       <c r="D16">
-        <v>870</v>
+        <v>915</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
       </c>
       <c r="C17">
-        <v>810</v>
+        <v>795</v>
       </c>
       <c r="D17">
-        <v>870</v>
+        <v>855</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
       </c>
       <c r="C18">
-        <v>810</v>
+        <v>795</v>
       </c>
       <c r="D18">
-        <v>870</v>
+        <v>855</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
         <v>6</v>
       </c>
       <c r="C19">
-        <v>810</v>
+        <v>795</v>
       </c>
       <c r="D19">
-        <v>870</v>
+        <v>855</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
         <v>9</v>
       </c>
       <c r="C20">
-        <v>960</v>
+        <v>855</v>
       </c>
       <c r="D20">
-        <v>1020</v>
+        <v>915</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B21" t="s">
         <v>9</v>
       </c>
       <c r="C21">
-        <v>960</v>
+        <v>855</v>
       </c>
       <c r="D21">
-        <v>1020</v>
+        <v>915</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
         <v>5</v>
       </c>
       <c r="C22">
-        <v>885</v>
+        <v>540</v>
       </c>
       <c r="D22">
-        <v>945</v>
+        <v>600</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
       </c>
       <c r="C23">
-        <v>540</v>
+        <v>795</v>
       </c>
       <c r="D23">
-        <v>600</v>
+        <v>855</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
         <v>5</v>
       </c>
       <c r="C24">
-        <v>540</v>
+        <v>795</v>
       </c>
       <c r="D24">
-        <v>600</v>
+        <v>855</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C25">
-        <v>960</v>
+        <v>795</v>
       </c>
       <c r="D25">
-        <v>1020</v>
+        <v>855</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B26" t="s">
         <v>6</v>
       </c>
       <c r="C26">
-        <v>885</v>
+        <v>855</v>
       </c>
       <c r="D26">
-        <v>945</v>
+        <v>915</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>9</v>
       </c>
       <c r="C27">
-        <v>540</v>
+        <v>795</v>
       </c>
       <c r="D27">
-        <v>600</v>
+        <v>855</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C28">
-        <v>690</v>
+        <v>855</v>
       </c>
       <c r="D28">
-        <v>750</v>
+        <v>915</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B29" t="s">
         <v>5</v>
       </c>
       <c r="C29">
-        <v>810</v>
+        <v>855</v>
       </c>
       <c r="D29">
-        <v>870</v>
+        <v>915</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B30" t="s">
         <v>6</v>
       </c>
       <c r="C30">
-        <v>615</v>
+        <v>930</v>
       </c>
       <c r="D30">
-        <v>675</v>
+        <v>990</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B31" t="s">
         <v>7</v>
       </c>
       <c r="C31">
-        <v>885</v>
+        <v>540</v>
       </c>
       <c r="D31">
-        <v>945</v>
+        <v>600</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B32" t="s">
         <v>5</v>
       </c>
       <c r="C32">
-        <v>810</v>
+        <v>855</v>
       </c>
       <c r="D32">
-        <v>870</v>
+        <v>915</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B33" t="s">
         <v>6</v>
       </c>
       <c r="C33">
-        <v>615</v>
+        <v>930</v>
       </c>
       <c r="D33">
-        <v>675</v>
+        <v>990</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B34" t="s">
         <v>7</v>
       </c>
       <c r="C34">
-        <v>885</v>
+        <v>540</v>
       </c>
       <c r="D34">
-        <v>945</v>
+        <v>600</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B35" t="s">
         <v>6</v>
       </c>
       <c r="C35">
-        <v>885</v>
+        <v>855</v>
       </c>
       <c r="D35">
-        <v>945</v>
+        <v>915</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B36" t="s">
         <v>9</v>
       </c>
       <c r="C36">
-        <v>540</v>
+        <v>795</v>
       </c>
       <c r="D36">
-        <v>600</v>
+        <v>855</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B37" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C37">
-        <v>690</v>
+        <v>855</v>
       </c>
       <c r="D37">
-        <v>750</v>
+        <v>915</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B38" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C38">
         <v>615</v>
@@ -1204,30 +1204,30 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B39" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C39">
-        <v>810</v>
+        <v>540</v>
       </c>
       <c r="D39">
-        <v>870</v>
+        <v>600</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B40" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="C40">
-        <v>540</v>
+        <v>480</v>
       </c>
       <c r="D40">
-        <v>600</v>
+        <v>540</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1235,7 +1235,7 @@
         <v>31</v>
       </c>
       <c r="B41" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C41">
         <v>615</v>
@@ -1249,13 +1249,13 @@
         <v>31</v>
       </c>
       <c r="B42" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C42">
-        <v>810</v>
+        <v>540</v>
       </c>
       <c r="D42">
-        <v>870</v>
+        <v>600</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1263,13 +1263,13 @@
         <v>31</v>
       </c>
       <c r="B43" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="C43">
-        <v>540</v>
+        <v>480</v>
       </c>
       <c r="D43">
-        <v>600</v>
+        <v>540</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1280,10 +1280,10 @@
         <v>5</v>
       </c>
       <c r="C44">
-        <v>960</v>
+        <v>615</v>
       </c>
       <c r="D44">
-        <v>1020</v>
+        <v>675</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1291,13 +1291,13 @@
         <v>33</v>
       </c>
       <c r="B45" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C45">
-        <v>960</v>
+        <v>795</v>
       </c>
       <c r="D45">
-        <v>1020</v>
+        <v>855</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1305,13 +1305,13 @@
         <v>34</v>
       </c>
       <c r="B46" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C46">
-        <v>810</v>
+        <v>855</v>
       </c>
       <c r="D46">
-        <v>870</v>
+        <v>915</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1319,13 +1319,13 @@
         <v>35</v>
       </c>
       <c r="B47" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C47">
-        <v>960</v>
+        <v>795</v>
       </c>
       <c r="D47">
-        <v>1020</v>
+        <v>855</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1336,10 +1336,10 @@
         <v>6</v>
       </c>
       <c r="C48">
-        <v>810</v>
+        <v>795</v>
       </c>
       <c r="D48">
-        <v>870</v>
+        <v>855</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1350,10 +1350,10 @@
         <v>5</v>
       </c>
       <c r="C49">
-        <v>960</v>
+        <v>615</v>
       </c>
       <c r="D49">
-        <v>1020</v>
+        <v>675</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1364,10 +1364,10 @@
         <v>6</v>
       </c>
       <c r="C50">
-        <v>810</v>
+        <v>795</v>
       </c>
       <c r="D50">
-        <v>870</v>
+        <v>855</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1375,7 +1375,7 @@
         <v>39</v>
       </c>
       <c r="B51" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C51">
         <v>615</v>
@@ -1389,13 +1389,13 @@
         <v>39</v>
       </c>
       <c r="B52" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C52">
-        <v>810</v>
+        <v>540</v>
       </c>
       <c r="D52">
-        <v>870</v>
+        <v>600</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1403,13 +1403,13 @@
         <v>39</v>
       </c>
       <c r="B53" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="C53">
-        <v>540</v>
+        <v>480</v>
       </c>
       <c r="D53">
-        <v>600</v>
+        <v>540</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -1420,10 +1420,10 @@
         <v>5</v>
       </c>
       <c r="C54">
-        <v>960</v>
+        <v>615</v>
       </c>
       <c r="D54">
-        <v>1020</v>
+        <v>675</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -1431,7 +1431,7 @@
         <v>41</v>
       </c>
       <c r="B55" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C55">
         <v>615</v>
@@ -1445,13 +1445,13 @@
         <v>41</v>
       </c>
       <c r="B56" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C56">
-        <v>810</v>
+        <v>540</v>
       </c>
       <c r="D56">
-        <v>870</v>
+        <v>600</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -1459,13 +1459,13 @@
         <v>41</v>
       </c>
       <c r="B57" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="C57">
-        <v>540</v>
+        <v>480</v>
       </c>
       <c r="D57">
-        <v>600</v>
+        <v>540</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -1490,10 +1490,10 @@
         <v>5</v>
       </c>
       <c r="C59">
-        <v>960</v>
+        <v>615</v>
       </c>
       <c r="D59">
-        <v>1020</v>
+        <v>675</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -1514,10 +1514,10 @@
         <v>9</v>
       </c>
       <c r="C62">
-        <v>615</v>
+        <v>540</v>
       </c>
       <c r="D62">
-        <v>675</v>
+        <v>600</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -1525,13 +1525,13 @@
         <v>46</v>
       </c>
       <c r="B63" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C63">
-        <v>615</v>
+        <v>795</v>
       </c>
       <c r="D63">
-        <v>675</v>
+        <v>855</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -1539,13 +1539,13 @@
         <v>46</v>
       </c>
       <c r="B64" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="C64">
-        <v>615</v>
+        <v>675</v>
       </c>
       <c r="D64">
-        <v>675</v>
+        <v>735</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -1556,10 +1556,10 @@
         <v>9</v>
       </c>
       <c r="C65">
-        <v>615</v>
+        <v>540</v>
       </c>
       <c r="D65">
-        <v>675</v>
+        <v>600</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -1567,13 +1567,13 @@
         <v>47</v>
       </c>
       <c r="B66" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C66">
-        <v>615</v>
+        <v>795</v>
       </c>
       <c r="D66">
-        <v>675</v>
+        <v>855</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -1581,13 +1581,13 @@
         <v>47</v>
       </c>
       <c r="B67" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="C67">
-        <v>615</v>
+        <v>675</v>
       </c>
       <c r="D67">
-        <v>675</v>
+        <v>735</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -1612,10 +1612,10 @@
         <v>5</v>
       </c>
       <c r="C69">
-        <v>885</v>
+        <v>540</v>
       </c>
       <c r="D69">
-        <v>945</v>
+        <v>600</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -1640,10 +1640,10 @@
         <v>5</v>
       </c>
       <c r="C71">
-        <v>540</v>
+        <v>795</v>
       </c>
       <c r="D71">
-        <v>600</v>
+        <v>855</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -1651,13 +1651,13 @@
         <v>52</v>
       </c>
       <c r="B72" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C72">
-        <v>885</v>
+        <v>615</v>
       </c>
       <c r="D72">
-        <v>945</v>
+        <v>675</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -1665,13 +1665,13 @@
         <v>53</v>
       </c>
       <c r="B73" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C73">
-        <v>885</v>
+        <v>540</v>
       </c>
       <c r="D73">
-        <v>945</v>
+        <v>600</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -1682,10 +1682,10 @@
         <v>9</v>
       </c>
       <c r="C74">
-        <v>615</v>
+        <v>540</v>
       </c>
       <c r="D74">
-        <v>675</v>
+        <v>600</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -1693,13 +1693,13 @@
         <v>54</v>
       </c>
       <c r="B75" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C75">
-        <v>615</v>
+        <v>795</v>
       </c>
       <c r="D75">
-        <v>675</v>
+        <v>855</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -1707,13 +1707,13 @@
         <v>54</v>
       </c>
       <c r="B76" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="C76">
-        <v>615</v>
+        <v>675</v>
       </c>
       <c r="D76">
-        <v>675</v>
+        <v>735</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -1721,13 +1721,13 @@
         <v>55</v>
       </c>
       <c r="B77" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C77">
-        <v>960</v>
+        <v>540</v>
       </c>
       <c r="D77">
-        <v>1020</v>
+        <v>600</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -1749,13 +1749,13 @@
         <v>57</v>
       </c>
       <c r="B79" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C79">
-        <v>885</v>
+        <v>615</v>
       </c>
       <c r="D79">
-        <v>945</v>
+        <v>675</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -1763,13 +1763,13 @@
         <v>58</v>
       </c>
       <c r="B80" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C80">
-        <v>885</v>
+        <v>540</v>
       </c>
       <c r="D80">
-        <v>945</v>
+        <v>600</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -1780,10 +1780,10 @@
         <v>9</v>
       </c>
       <c r="C81">
-        <v>615</v>
+        <v>540</v>
       </c>
       <c r="D81">
-        <v>675</v>
+        <v>600</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -1791,13 +1791,13 @@
         <v>59</v>
       </c>
       <c r="B82" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C82">
-        <v>615</v>
+        <v>795</v>
       </c>
       <c r="D82">
-        <v>675</v>
+        <v>855</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -1805,24 +1805,42 @@
         <v>59</v>
       </c>
       <c r="B83" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="C83">
-        <v>615</v>
+        <v>675</v>
       </c>
       <c r="D83">
-        <v>675</v>
+        <v>735</v>
       </c>
     </row>
     <row r="84" spans="1:4">
       <c r="A84" t="s">
         <v>60</v>
       </c>
+      <c r="B84" t="s">
+        <v>14</v>
+      </c>
+      <c r="C84">
+        <v>540</v>
+      </c>
+      <c r="D84">
+        <v>600</v>
+      </c>
     </row>
     <row r="85" spans="1:4">
       <c r="A85" t="s">
         <v>61</v>
       </c>
+      <c r="B85" t="s">
+        <v>7</v>
+      </c>
+      <c r="C85">
+        <v>615</v>
+      </c>
+      <c r="D85">
+        <v>675</v>
+      </c>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" t="s">
@@ -1832,10 +1850,10 @@
         <v>5</v>
       </c>
       <c r="C86">
-        <v>690</v>
+        <v>675</v>
       </c>
       <c r="D86">
-        <v>750</v>
+        <v>735</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -1846,10 +1864,10 @@
         <v>6</v>
       </c>
       <c r="C87">
-        <v>690</v>
+        <v>675</v>
       </c>
       <c r="D87">
-        <v>750</v>
+        <v>735</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -1860,10 +1878,10 @@
         <v>9</v>
       </c>
       <c r="C88">
-        <v>690</v>
+        <v>675</v>
       </c>
       <c r="D88">
-        <v>750</v>
+        <v>735</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -1874,10 +1892,10 @@
         <v>5</v>
       </c>
       <c r="C89">
-        <v>690</v>
+        <v>675</v>
       </c>
       <c r="D89">
-        <v>750</v>
+        <v>735</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -1888,10 +1906,10 @@
         <v>6</v>
       </c>
       <c r="C90">
-        <v>690</v>
+        <v>675</v>
       </c>
       <c r="D90">
-        <v>750</v>
+        <v>735</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -1902,10 +1920,10 @@
         <v>9</v>
       </c>
       <c r="C91">
-        <v>690</v>
+        <v>675</v>
       </c>
       <c r="D91">
-        <v>750</v>
+        <v>735</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -1916,10 +1934,10 @@
         <v>5</v>
       </c>
       <c r="C92">
-        <v>690</v>
+        <v>675</v>
       </c>
       <c r="D92">
-        <v>750</v>
+        <v>735</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -1930,10 +1948,10 @@
         <v>6</v>
       </c>
       <c r="C93">
-        <v>690</v>
+        <v>675</v>
       </c>
       <c r="D93">
-        <v>750</v>
+        <v>735</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -1944,10 +1962,10 @@
         <v>9</v>
       </c>
       <c r="C94">
-        <v>690</v>
+        <v>675</v>
       </c>
       <c r="D94">
-        <v>750</v>
+        <v>735</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -1958,10 +1976,10 @@
         <v>5</v>
       </c>
       <c r="C95">
-        <v>690</v>
+        <v>675</v>
       </c>
       <c r="D95">
-        <v>750</v>
+        <v>735</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -1972,10 +1990,10 @@
         <v>6</v>
       </c>
       <c r="C96">
-        <v>690</v>
+        <v>675</v>
       </c>
       <c r="D96">
-        <v>750</v>
+        <v>735</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -1986,10 +2004,10 @@
         <v>9</v>
       </c>
       <c r="C97">
-        <v>690</v>
+        <v>675</v>
       </c>
       <c r="D97">
-        <v>750</v>
+        <v>735</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -2000,10 +2018,10 @@
         <v>5</v>
       </c>
       <c r="C98">
-        <v>690</v>
+        <v>675</v>
       </c>
       <c r="D98">
-        <v>750</v>
+        <v>735</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -2014,10 +2032,10 @@
         <v>6</v>
       </c>
       <c r="C99">
-        <v>690</v>
+        <v>675</v>
       </c>
       <c r="D99">
-        <v>750</v>
+        <v>735</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -2028,10 +2046,10 @@
         <v>9</v>
       </c>
       <c r="C100">
-        <v>690</v>
+        <v>675</v>
       </c>
       <c r="D100">
-        <v>750</v>
+        <v>735</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -2042,10 +2060,10 @@
         <v>5</v>
       </c>
       <c r="C101">
-        <v>690</v>
+        <v>675</v>
       </c>
       <c r="D101">
-        <v>750</v>
+        <v>735</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -2056,10 +2074,10 @@
         <v>6</v>
       </c>
       <c r="C102">
-        <v>690</v>
+        <v>675</v>
       </c>
       <c r="D102">
-        <v>750</v>
+        <v>735</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -2070,10 +2088,10 @@
         <v>9</v>
       </c>
       <c r="C103">
-        <v>690</v>
+        <v>675</v>
       </c>
       <c r="D103">
-        <v>750</v>
+        <v>735</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -2084,10 +2102,10 @@
         <v>5</v>
       </c>
       <c r="C104">
-        <v>690</v>
+        <v>675</v>
       </c>
       <c r="D104">
-        <v>750</v>
+        <v>735</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -2098,10 +2116,10 @@
         <v>6</v>
       </c>
       <c r="C105">
-        <v>690</v>
+        <v>675</v>
       </c>
       <c r="D105">
-        <v>750</v>
+        <v>735</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -2112,10 +2130,10 @@
         <v>9</v>
       </c>
       <c r="C106">
-        <v>690</v>
+        <v>675</v>
       </c>
       <c r="D106">
-        <v>750</v>
+        <v>735</v>
       </c>
     </row>
     <row r="107" spans="1:4">
@@ -2123,13 +2141,13 @@
         <v>69</v>
       </c>
       <c r="B107" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C107">
-        <v>540</v>
+        <v>615</v>
       </c>
       <c r="D107">
-        <v>600</v>
+        <v>675</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -2137,13 +2155,13 @@
         <v>69</v>
       </c>
       <c r="B108" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C108">
-        <v>615</v>
+        <v>675</v>
       </c>
       <c r="D108">
-        <v>675</v>
+        <v>735</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -2151,13 +2169,13 @@
         <v>70</v>
       </c>
       <c r="B109" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C109">
-        <v>540</v>
+        <v>615</v>
       </c>
       <c r="D109">
-        <v>600</v>
+        <v>675</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -2165,13 +2183,13 @@
         <v>70</v>
       </c>
       <c r="B110" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C110">
-        <v>615</v>
+        <v>675</v>
       </c>
       <c r="D110">
-        <v>675</v>
+        <v>735</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -2182,10 +2200,10 @@
         <v>5</v>
       </c>
       <c r="C111">
-        <v>885</v>
+        <v>540</v>
       </c>
       <c r="D111">
-        <v>945</v>
+        <v>600</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -2196,10 +2214,10 @@
         <v>9</v>
       </c>
       <c r="C112">
-        <v>810</v>
+        <v>615</v>
       </c>
       <c r="D112">
-        <v>870</v>
+        <v>675</v>
       </c>
     </row>
     <row r="113" spans="1:4">
@@ -2207,13 +2225,13 @@
         <v>73</v>
       </c>
       <c r="B113" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C113">
-        <v>540</v>
+        <v>615</v>
       </c>
       <c r="D113">
-        <v>600</v>
+        <v>675</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -2221,13 +2239,13 @@
         <v>74</v>
       </c>
       <c r="B114" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C114">
-        <v>690</v>
+        <v>675</v>
       </c>
       <c r="D114">
-        <v>750</v>
+        <v>735</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -2235,13 +2253,13 @@
         <v>75</v>
       </c>
       <c r="B115" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C115">
-        <v>810</v>
+        <v>855</v>
       </c>
       <c r="D115">
-        <v>870</v>
+        <v>915</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -2249,13 +2267,13 @@
         <v>76</v>
       </c>
       <c r="B116" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C116">
-        <v>690</v>
+        <v>675</v>
       </c>
       <c r="D116">
-        <v>750</v>
+        <v>735</v>
       </c>
     </row>
     <row r="117" spans="1:4">
@@ -2263,13 +2281,13 @@
         <v>77</v>
       </c>
       <c r="B117" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C117">
-        <v>540</v>
+        <v>615</v>
       </c>
       <c r="D117">
-        <v>600</v>
+        <v>675</v>
       </c>
     </row>
     <row r="118" spans="1:4">
@@ -2277,13 +2295,13 @@
         <v>77</v>
       </c>
       <c r="B118" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C118">
-        <v>615</v>
+        <v>675</v>
       </c>
       <c r="D118">
-        <v>675</v>
+        <v>735</v>
       </c>
     </row>
     <row r="119" spans="1:4">
@@ -2294,10 +2312,10 @@
         <v>9</v>
       </c>
       <c r="C119">
-        <v>810</v>
+        <v>615</v>
       </c>
       <c r="D119">
-        <v>870</v>
+        <v>675</v>
       </c>
     </row>
     <row r="120" spans="1:4">
@@ -2305,13 +2323,13 @@
         <v>79</v>
       </c>
       <c r="B120" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C120">
-        <v>540</v>
+        <v>615</v>
       </c>
       <c r="D120">
-        <v>600</v>
+        <v>675</v>
       </c>
     </row>
     <row r="121" spans="1:4">
@@ -2319,13 +2337,13 @@
         <v>80</v>
       </c>
       <c r="B121" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C121">
-        <v>690</v>
+        <v>675</v>
       </c>
       <c r="D121">
-        <v>750</v>
+        <v>735</v>
       </c>
     </row>
     <row r="122" spans="1:4">
@@ -2333,13 +2351,13 @@
         <v>81</v>
       </c>
       <c r="B122" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C122">
-        <v>540</v>
+        <v>615</v>
       </c>
       <c r="D122">
-        <v>600</v>
+        <v>675</v>
       </c>
     </row>
     <row r="123" spans="1:4">
@@ -2347,13 +2365,13 @@
         <v>81</v>
       </c>
       <c r="B123" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C123">
-        <v>615</v>
+        <v>675</v>
       </c>
       <c r="D123">
-        <v>675</v>
+        <v>735</v>
       </c>
     </row>
     <row r="124" spans="1:4">
@@ -2364,10 +2382,10 @@
         <v>9</v>
       </c>
       <c r="C124">
-        <v>810</v>
+        <v>615</v>
       </c>
       <c r="D124">
-        <v>870</v>
+        <v>675</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -2375,13 +2393,13 @@
         <v>83</v>
       </c>
       <c r="B125" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C125">
-        <v>540</v>
+        <v>615</v>
       </c>
       <c r="D125">
-        <v>600</v>
+        <v>675</v>
       </c>
     </row>
     <row r="126" spans="1:4">
@@ -2389,13 +2407,13 @@
         <v>84</v>
       </c>
       <c r="B126" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C126">
-        <v>690</v>
+        <v>675</v>
       </c>
       <c r="D126">
-        <v>750</v>
+        <v>735</v>
       </c>
     </row>
     <row r="127" spans="1:4">
@@ -2403,13 +2421,13 @@
         <v>85</v>
       </c>
       <c r="B127" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="C127">
-        <v>810</v>
+        <v>735</v>
       </c>
       <c r="D127">
-        <v>870</v>
+        <v>915</v>
       </c>
     </row>
   </sheetData>
@@ -2421,7 +2439,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F36BBCB0-0C4B-4DF4-ACEE-CB158947AE36}">
   <dimension ref="A1:I130"/>
   <sheetViews>
-    <sheetView topLeftCell="A74" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F105" sqref="F105"/>
     </sheetView>
   </sheetViews>
@@ -2450,7 +2468,7 @@
         <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2">
         <v>540</v>
@@ -2464,7 +2482,7 @@
         <v>79</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3">
         <v>540</v>
@@ -2478,7 +2496,7 @@
         <v>83</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4">
         <v>540</v>
@@ -2492,7 +2510,7 @@
         <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5">
         <v>615</v>
@@ -2506,7 +2524,7 @@
         <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6">
         <v>615</v>
@@ -2520,7 +2538,7 @@
         <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7">
         <v>615</v>
@@ -2534,7 +2552,7 @@
         <v>59</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C8">
         <v>615</v>
@@ -2548,7 +2566,7 @@
         <v>74</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C9">
         <v>690</v>
@@ -2562,7 +2580,7 @@
         <v>76</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C10">
         <v>690</v>
@@ -2576,7 +2594,7 @@
         <v>80</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C11">
         <v>690</v>
@@ -2590,7 +2608,7 @@
         <v>84</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C12">
         <v>690</v>
@@ -2601,10 +2619,10 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C13">
         <v>810</v>
@@ -2615,10 +2633,10 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
         <v>14</v>
-      </c>
-      <c r="B14" t="s">
-        <v>13</v>
       </c>
       <c r="C14">
         <v>810</v>
@@ -2629,10 +2647,10 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C15">
         <v>810</v>
@@ -2646,7 +2664,7 @@
         <v>34</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C16">
         <v>810</v>
@@ -2660,7 +2678,7 @@
         <v>75</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C17">
         <v>810</v>
@@ -2674,7 +2692,7 @@
         <v>53</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C18">
         <v>885</v>
@@ -2688,7 +2706,7 @@
         <v>58</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C19">
         <v>885</v>
@@ -2699,7 +2717,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B20" t="s">
         <v>5</v>
@@ -2713,7 +2731,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B21" t="s">
         <v>5</v>
@@ -2741,7 +2759,7 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -2923,7 +2941,7 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B36" t="s">
         <v>5</v>
@@ -2937,7 +2955,7 @@
     </row>
     <row r="37" spans="1:9">
       <c r="A37" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B37" t="s">
         <v>5</v>
@@ -2951,7 +2969,7 @@
     </row>
     <row r="38" spans="1:9">
       <c r="A38" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B38" t="s">
         <v>5</v>
@@ -2965,7 +2983,7 @@
     </row>
     <row r="39" spans="1:9">
       <c r="A39" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B39" t="s">
         <v>5</v>
@@ -3063,10 +3081,10 @@
     </row>
     <row r="46" spans="1:9">
       <c r="A46" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B46" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="C46">
         <v>540</v>
@@ -3080,7 +3098,7 @@
         <v>31</v>
       </c>
       <c r="B47" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="C47">
         <v>540</v>
@@ -3095,7 +3113,7 @@
         <v>39</v>
       </c>
       <c r="B48" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="C48">
         <v>540</v>
@@ -3110,7 +3128,7 @@
         <v>41</v>
       </c>
       <c r="B49" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="C49">
         <v>540</v>
@@ -3125,7 +3143,7 @@
         <v>46</v>
       </c>
       <c r="B50" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="C50">
         <v>615</v>
@@ -3140,7 +3158,7 @@
         <v>47</v>
       </c>
       <c r="B51" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="C51">
         <v>615</v>
@@ -3155,7 +3173,7 @@
         <v>54</v>
       </c>
       <c r="B52" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="C52">
         <v>615</v>
@@ -3170,7 +3188,7 @@
         <v>59</v>
       </c>
       <c r="B53" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="C53">
         <v>615</v>
@@ -3185,7 +3203,7 @@
         <v>85</v>
       </c>
       <c r="B54" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="C54">
         <v>810</v>
@@ -3200,7 +3218,7 @@
         <v>69</v>
       </c>
       <c r="B55" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C55">
         <v>540</v>
@@ -3215,7 +3233,7 @@
         <v>70</v>
       </c>
       <c r="B56" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C56">
         <v>540</v>
@@ -3230,7 +3248,7 @@
         <v>77</v>
       </c>
       <c r="B57" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C57">
         <v>540</v>
@@ -3245,7 +3263,7 @@
         <v>81</v>
       </c>
       <c r="B58" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C58">
         <v>540</v>
@@ -3260,7 +3278,7 @@
         <v>69</v>
       </c>
       <c r="B59" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C59">
         <v>615</v>
@@ -3275,7 +3293,7 @@
         <v>70</v>
       </c>
       <c r="B60" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C60">
         <v>615</v>
@@ -3290,7 +3308,7 @@
         <v>77</v>
       </c>
       <c r="B61" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C61">
         <v>615</v>
@@ -3305,7 +3323,7 @@
         <v>81</v>
       </c>
       <c r="B62" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C62">
         <v>615</v>
@@ -3320,7 +3338,7 @@
         <v>8</v>
       </c>
       <c r="B63" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C63">
         <v>690</v>
@@ -3332,10 +3350,10 @@
     </row>
     <row r="64" spans="1:9">
       <c r="A64" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B64" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C64">
         <v>690</v>
@@ -3347,10 +3365,10 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B65" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C65">
         <v>690</v>
@@ -3361,10 +3379,10 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B66" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C66">
         <v>690</v>
@@ -3375,10 +3393,10 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B67" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C67">
         <v>810</v>
@@ -3392,7 +3410,7 @@
         <v>31</v>
       </c>
       <c r="B68" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C68">
         <v>810</v>
@@ -3406,7 +3424,7 @@
         <v>39</v>
       </c>
       <c r="B69" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C69">
         <v>810</v>
@@ -3420,7 +3438,7 @@
         <v>41</v>
       </c>
       <c r="B70" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C70">
         <v>810</v>
@@ -3434,7 +3452,7 @@
         <v>4</v>
       </c>
       <c r="B71" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C71">
         <v>885</v>
@@ -3445,10 +3463,10 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B72" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C72">
         <v>885</v>
@@ -3459,10 +3477,10 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B73" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C73">
         <v>885</v>
@@ -3473,10 +3491,10 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B74" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C74">
         <v>885</v>
@@ -3487,10 +3505,10 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B75" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C75">
         <v>960</v>
@@ -3504,7 +3522,7 @@
         <v>35</v>
       </c>
       <c r="B76" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C76">
         <v>960</v>
@@ -3518,7 +3536,7 @@
         <v>55</v>
       </c>
       <c r="B77" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C77">
         <v>960</v>
@@ -3585,7 +3603,7 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B82" t="s">
         <v>6</v>
@@ -3599,7 +3617,7 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B83" t="s">
         <v>6</v>
@@ -3613,7 +3631,7 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B84" t="s">
         <v>6</v>
@@ -3739,7 +3757,7 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B93" t="s">
         <v>6</v>
@@ -3753,7 +3771,7 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B94" t="s">
         <v>6</v>
@@ -3767,7 +3785,7 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B95" t="s">
         <v>6</v>
@@ -3823,7 +3841,7 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B99" t="s">
         <v>6</v>
@@ -3837,7 +3855,7 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B100" t="s">
         <v>6</v>
@@ -3851,7 +3869,7 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B101" t="s">
         <v>6</v>
@@ -3879,7 +3897,7 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B103" t="s">
         <v>9</v>
@@ -3893,7 +3911,7 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B104" t="s">
         <v>9</v>
@@ -3907,7 +3925,7 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B105" t="s">
         <v>9</v>
@@ -4159,7 +4177,7 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B123" t="s">
         <v>9</v>
@@ -4173,7 +4191,7 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B124" t="s">
         <v>9</v>
@@ -4246,9 +4264,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB565AE7-DA39-4EFA-AE27-F4B506899741}">
   <dimension ref="A1:F127"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F127"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -4299,7 +4315,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C4">
         <v>885</v>
@@ -4341,7 +4357,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C7">
         <v>690</v>
@@ -4352,7 +4368,7 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -4366,7 +4382,7 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
@@ -4380,10 +4396,10 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C10">
         <v>690</v>
@@ -4394,7 +4410,7 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
@@ -4411,7 +4427,7 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
@@ -4428,10 +4444,10 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C13">
         <v>885</v>
@@ -4445,10 +4461,10 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C14">
         <v>810</v>
@@ -4459,10 +4475,10 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
         <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>13</v>
       </c>
       <c r="C15">
         <v>810</v>
@@ -4473,10 +4489,10 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C16">
         <v>810</v>
@@ -4487,7 +4503,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
@@ -4501,7 +4517,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
@@ -4515,7 +4531,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
         <v>6</v>
@@ -4529,7 +4545,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
         <v>9</v>
@@ -4543,7 +4559,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B21" t="s">
         <v>9</v>
@@ -4557,7 +4573,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
         <v>5</v>
@@ -4571,7 +4587,7 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -4585,7 +4601,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
         <v>5</v>
@@ -4599,10 +4615,10 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C25">
         <v>960</v>
@@ -4613,7 +4629,7 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B26" t="s">
         <v>6</v>
@@ -4627,7 +4643,7 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>9</v>
@@ -4641,10 +4657,10 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C28">
         <v>690</v>
@@ -4655,7 +4671,7 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B29" t="s">
         <v>5</v>
@@ -4669,7 +4685,7 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B30" t="s">
         <v>6</v>
@@ -4683,10 +4699,10 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B31" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C31">
         <v>885</v>
@@ -4697,7 +4713,7 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B32" t="s">
         <v>5</v>
@@ -4711,7 +4727,7 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B33" t="s">
         <v>6</v>
@@ -4725,10 +4741,10 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B34" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C34">
         <v>885</v>
@@ -4739,7 +4755,7 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B35" t="s">
         <v>6</v>
@@ -4756,7 +4772,7 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B36" t="s">
         <v>9</v>
@@ -4773,10 +4789,10 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B37" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C37">
         <v>690</v>
@@ -4790,7 +4806,7 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B38" t="s">
         <v>5</v>
@@ -4807,10 +4823,10 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B39" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C39">
         <v>810</v>
@@ -4824,10 +4840,10 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B40" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="C40">
         <v>540</v>
@@ -4858,7 +4874,7 @@
         <v>31</v>
       </c>
       <c r="B42" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C42">
         <v>810</v>
@@ -4872,7 +4888,7 @@
         <v>31</v>
       </c>
       <c r="B43" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="C43">
         <v>540</v>
@@ -4914,7 +4930,7 @@
         <v>34</v>
       </c>
       <c r="B46" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C46">
         <v>810</v>
@@ -4928,7 +4944,7 @@
         <v>35</v>
       </c>
       <c r="B47" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C47">
         <v>960</v>
@@ -5001,7 +5017,7 @@
         <v>39</v>
       </c>
       <c r="B52" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C52">
         <v>810</v>
@@ -5015,7 +5031,7 @@
         <v>39</v>
       </c>
       <c r="B53" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="C53">
         <v>540</v>
@@ -5057,7 +5073,7 @@
         <v>41</v>
       </c>
       <c r="B56" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C56">
         <v>810</v>
@@ -5071,7 +5087,7 @@
         <v>41</v>
       </c>
       <c r="B57" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="C57">
         <v>540</v>
@@ -5137,7 +5153,7 @@
         <v>46</v>
       </c>
       <c r="B63" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C63">
         <v>615</v>
@@ -5151,7 +5167,7 @@
         <v>46</v>
       </c>
       <c r="B64" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="C64">
         <v>615</v>
@@ -5179,7 +5195,7 @@
         <v>47</v>
       </c>
       <c r="B66" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C66">
         <v>615</v>
@@ -5193,7 +5209,7 @@
         <v>47</v>
       </c>
       <c r="B67" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="C67">
         <v>615</v>
@@ -5277,7 +5293,7 @@
         <v>53</v>
       </c>
       <c r="B73" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C73">
         <v>885</v>
@@ -5305,7 +5321,7 @@
         <v>54</v>
       </c>
       <c r="B75" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C75">
         <v>615</v>
@@ -5319,7 +5335,7 @@
         <v>54</v>
       </c>
       <c r="B76" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="C76">
         <v>615</v>
@@ -5333,7 +5349,7 @@
         <v>55</v>
       </c>
       <c r="B77" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C77">
         <v>960</v>
@@ -5381,7 +5397,7 @@
         <v>58</v>
       </c>
       <c r="B80" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C80">
         <v>885</v>
@@ -5415,7 +5431,7 @@
         <v>59</v>
       </c>
       <c r="B82" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C82">
         <v>615</v>
@@ -5432,7 +5448,7 @@
         <v>59</v>
       </c>
       <c r="B83" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="C83">
         <v>615</v>
@@ -5771,7 +5787,7 @@
         <v>69</v>
       </c>
       <c r="B107" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C107">
         <v>540</v>
@@ -5788,7 +5804,7 @@
         <v>69</v>
       </c>
       <c r="B108" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C108">
         <v>615</v>
@@ -5805,7 +5821,7 @@
         <v>70</v>
       </c>
       <c r="B109" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C109">
         <v>540</v>
@@ -5822,7 +5838,7 @@
         <v>70</v>
       </c>
       <c r="B110" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C110">
         <v>615</v>
@@ -5867,7 +5883,7 @@
         <v>73</v>
       </c>
       <c r="B113" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C113">
         <v>540</v>
@@ -5881,7 +5897,7 @@
         <v>74</v>
       </c>
       <c r="B114" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C114">
         <v>690</v>
@@ -5895,7 +5911,7 @@
         <v>75</v>
       </c>
       <c r="B115" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C115">
         <v>810</v>
@@ -5909,7 +5925,7 @@
         <v>76</v>
       </c>
       <c r="B116" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C116">
         <v>690</v>
@@ -5923,7 +5939,7 @@
         <v>77</v>
       </c>
       <c r="B117" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C117">
         <v>540</v>
@@ -5940,7 +5956,7 @@
         <v>77</v>
       </c>
       <c r="B118" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C118">
         <v>615</v>
@@ -5971,7 +5987,7 @@
         <v>79</v>
       </c>
       <c r="B120" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C120">
         <v>540</v>
@@ -5985,7 +6001,7 @@
         <v>80</v>
       </c>
       <c r="B121" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C121">
         <v>690</v>
@@ -5999,7 +6015,7 @@
         <v>81</v>
       </c>
       <c r="B122" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C122">
         <v>540</v>
@@ -6013,7 +6029,7 @@
         <v>81</v>
       </c>
       <c r="B123" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C123">
         <v>615</v>
@@ -6041,7 +6057,7 @@
         <v>83</v>
       </c>
       <c r="B125" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C125">
         <v>540</v>
@@ -6055,7 +6071,7 @@
         <v>84</v>
       </c>
       <c r="B126" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C126">
         <v>690</v>
@@ -6069,7 +6085,7 @@
         <v>85</v>
       </c>
       <c r="B127" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="C127">
         <v>810</v>

</xml_diff>